<commit_message>
new spell cards, and revamped player
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212CEC50-EFD0-4C90-A0B1-28767755EF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813A8CE-4B90-4CD7-B417-FDE4A861CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="18945" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Gain a :plant: when someone uses Windsharing</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Fireball</t>
   </si>
   <si>
@@ -294,12 +291,6 @@
     <t>Desc2</t>
   </si>
   <si>
-    <t>Place marker on Casino. Next roll you may modify the roll +/- 1.</t>
-  </si>
-  <si>
-    <t>PPFF</t>
-  </si>
-  <si>
     <t>Stacks</t>
   </si>
   <si>
@@ -316,6 +307,54 @@
   </si>
   <si>
     <t>Deal 2 damage. If this spell has two stacks, add Daze to boss feet.</t>
+  </si>
+  <si>
+    <t>Extinguish 1 Flame</t>
+  </si>
+  <si>
+    <t>Deal 5 damage to a single body part</t>
+  </si>
+  <si>
+    <t>Deal 3 damage to two different body parts</t>
+  </si>
+  <si>
+    <t>Hurricane</t>
+  </si>
+  <si>
+    <t>Squall</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>AAWWW</t>
+  </si>
+  <si>
+    <t>Deal 4 damage</t>
+  </si>
+  <si>
+    <t>Deal 3 damage. Deal 1 damage for each player who contributes an AW to this spell.</t>
+  </si>
+  <si>
+    <t>Rock Shield</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>Deal 2 damage</t>
+  </si>
+  <si>
+    <t>Place a marker on Casino for each stack. Your next Casino roll you may modify the roll +/- 1 for each marker.</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>For each stack, name a number 1-6. Roll a D6. If it equals one of your numbers, deal damage equal to the number of stacks.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -378,6 +417,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -718,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,8 +771,8 @@
     <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="57" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -738,65 +780,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>87</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2"/>
+      <c r="D2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" t="s">
-        <v>82</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4"/>
+      <c r="D4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -804,37 +850,90 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
+      <c r="D5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6"/>
+      <c r="D6" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
+      <c r="D10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
player updates, new spells
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813A8CE-4B90-4CD7-B417-FDE4A861CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE0870-7730-4984-B048-90FCA8A5AB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="18945" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spells" sheetId="1" r:id="rId1"/>
     <sheet name="Decipher" sheetId="2" r:id="rId2"/>
     <sheet name="Bonuses" sheetId="3" r:id="rId3"/>
-    <sheet name="Key" sheetId="4" r:id="rId4"/>
+    <sheet name="Weaknesses" sheetId="5" r:id="rId4"/>
+    <sheet name="Key" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="130">
   <si>
     <t>Name</t>
   </si>
@@ -306,15 +307,9 @@
     <t>Prevent 2 damage</t>
   </si>
   <si>
-    <t>Deal 2 damage. If this spell has two stacks, add Daze to boss feet.</t>
-  </si>
-  <si>
     <t>Extinguish 1 Flame</t>
   </si>
   <si>
-    <t>Deal 5 damage to a single body part</t>
-  </si>
-  <si>
     <t>Deal 3 damage to two different body parts</t>
   </si>
   <si>
@@ -351,10 +346,79 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>For each stack, name a number 1-6. Roll a D6. If it equals one of your numbers, deal damage equal to the number of stacks.</t>
+  </si>
+  <si>
+    <t>Spend 1 :air: to add 1 :fire: to this spell.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Gap in Armor</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Prevent 1 damage</t>
+  </si>
+  <si>
+    <t>At 2 Stacks, move Boss one space</t>
+  </si>
+  <si>
+    <t>Clay Hut</t>
+  </si>
+  <si>
+    <t>Gain 1 Worker</t>
+  </si>
+  <si>
+    <t>Deal 2 damage. At two stacks, add Daze to boss feet.</t>
+  </si>
+  <si>
+    <t>Daze two body parts</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Ultimate Sacrifice</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add 1 Worker from supply to this spell. Workers stay on this spell until cast. </t>
+  </si>
+  <si>
+    <t>Deal 1/2/4 Damage for 1/2/3 Workers. Workers are lost.</t>
+  </si>
+  <si>
+    <t>Add 1 Mage from supply to this spell. Mages stay on this spell until cast.</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Trebuchet</t>
+  </si>
+  <si>
+    <t>Deal 8 Damage if there are 3 mages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Boss is not in your town, deal 2 damage. </t>
+  </si>
+  <si>
+    <t>Deal 5 damage</t>
+  </si>
+  <si>
+    <t>If Boss is in your town, each other player may contribute 1 :stone: to this spell.</t>
   </si>
 </sst>
 </file>
@@ -760,16 +824,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="6"/>
@@ -786,7 +850,7 @@
         <v>87</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>86</v>
@@ -806,7 +870,7 @@
         <v>89</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -816,11 +880,14 @@
       <c r="B3" t="s">
         <v>78</v>
       </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
       <c r="D3" s="6" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -837,7 +904,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -865,10 +932,10 @@
         <v>84</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -879,21 +946,21 @@
         <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
@@ -902,29 +969,29 @@
         <v>88</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
@@ -933,7 +1000,75 @@
         <v>91</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1787,6 +1922,45 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE23D17-6C0D-456E-99EC-518CC53A97E5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C0A2EB-FB10-4574-98A0-D1F6D1D5A86D}">
   <dimension ref="A1:C17"/>
   <sheetViews>

</xml_diff>

<commit_message>
daily bonus cards, more player mods
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE0870-7730-4984-B048-90FCA8A5AB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35718355-B987-4D37-BB4F-43EBA5B6C804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spells" sheetId="1" r:id="rId1"/>
-    <sheet name="Decipher" sheetId="2" r:id="rId2"/>
-    <sheet name="Bonuses" sheetId="3" r:id="rId3"/>
-    <sheet name="Weaknesses" sheetId="5" r:id="rId4"/>
-    <sheet name="Key" sheetId="4" r:id="rId5"/>
+    <sheet name="Bonuses" sheetId="3" r:id="rId2"/>
+    <sheet name="Weaknesses" sheetId="5" r:id="rId3"/>
+    <sheet name="Key" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -52,21 +51,9 @@
     <t>F</t>
   </si>
   <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t>Col</t>
-  </si>
-  <si>
     <t>Bonus</t>
   </si>
   <si>
-    <t>FWWA</t>
-  </si>
-  <si>
-    <t>PPPP</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -109,9 +96,6 @@
     <t>Plant</t>
   </si>
   <si>
-    <t>RRL</t>
-  </si>
-  <si>
     <t>Balloon</t>
   </si>
   <si>
@@ -154,30 +138,6 @@
     <t>Sow</t>
   </si>
   <si>
-    <t>MMM</t>
-  </si>
-  <si>
-    <t>RLLLL</t>
-  </si>
-  <si>
-    <t>MEP</t>
-  </si>
-  <si>
-    <t>CLL</t>
-  </si>
-  <si>
-    <t>WWWW</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>BEE</t>
-  </si>
-  <si>
-    <t>ZZR</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -187,75 +147,15 @@
     <t>Bonus2</t>
   </si>
   <si>
-    <t>WW</t>
-  </si>
-  <si>
-    <t>RRLLL</t>
-  </si>
-  <si>
-    <t>PPF</t>
-  </si>
-  <si>
-    <t>MRLL</t>
-  </si>
-  <si>
-    <t>LLLLLL</t>
-  </si>
-  <si>
-    <t>WF</t>
-  </si>
-  <si>
     <t>AA</t>
   </si>
   <si>
-    <t>WAPFS</t>
-  </si>
-  <si>
-    <t>SSS</t>
-  </si>
-  <si>
-    <t>MMMR</t>
-  </si>
-  <si>
-    <t>MMRRL</t>
-  </si>
-  <si>
-    <t>RRRLL</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
-    <t>Player</t>
-  </si>
-  <si>
-    <t>Gain an :air: whenever you :hike:</t>
-  </si>
-  <si>
-    <t>Do not discard :fire: at the end of Overnight</t>
-  </si>
-  <si>
-    <t>At game start, fill in 2 Proteges</t>
-  </si>
-  <si>
-    <t>SWAP</t>
-  </si>
-  <si>
-    <t>SWPPP</t>
-  </si>
-  <si>
-    <t>SSWWW</t>
-  </si>
-  <si>
-    <t>SSWAA</t>
-  </si>
-  <si>
     <t>Economic Value</t>
   </si>
   <si>
-    <t>Gain a :plant: when someone uses Windsharing</t>
-  </si>
-  <si>
     <t>Fireball</t>
   </si>
   <si>
@@ -301,9 +201,6 @@
     <t>Deal 3 damage.</t>
   </si>
   <si>
-    <t>Move boss one space</t>
-  </si>
-  <si>
     <t>Prevent 2 damage</t>
   </si>
   <si>
@@ -382,36 +279,12 @@
     <t>Daze two body parts</t>
   </si>
   <si>
-    <t>Sacrifice</t>
-  </si>
-  <si>
-    <t>Ultimate Sacrifice</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add 1 Worker from supply to this spell. Workers stay on this spell until cast. </t>
-  </si>
-  <si>
-    <t>Deal 1/2/4 Damage for 1/2/3 Workers. Workers are lost.</t>
-  </si>
-  <si>
-    <t>Add 1 Mage from supply to this spell. Mages stay on this spell until cast.</t>
-  </si>
-  <si>
-    <t>WP</t>
-  </si>
-  <si>
     <t>AS</t>
   </si>
   <si>
     <t>Trebuchet</t>
   </si>
   <si>
-    <t>Deal 8 Damage if there are 3 mages.</t>
-  </si>
-  <si>
     <t xml:space="preserve">If Boss is not in your town, deal 2 damage. </t>
   </si>
   <si>
@@ -419,6 +292,129 @@
   </si>
   <si>
     <t>If Boss is in your town, each other player may contribute 1 :stone: to this spell.</t>
+  </si>
+  <si>
+    <t>Deal 1 damage. Move boss.</t>
+  </si>
+  <si>
+    <t>Feast</t>
+  </si>
+  <si>
+    <t>Gain 1 Mage</t>
+  </si>
+  <si>
+    <t>Rain Dance</t>
+  </si>
+  <si>
+    <t>AAFF</t>
+  </si>
+  <si>
+    <t>All players gain 1 :water:</t>
+  </si>
+  <si>
+    <t>Necromancy</t>
+  </si>
+  <si>
+    <t>AFWS</t>
+  </si>
+  <si>
+    <t>Gain 1 Mage recruitment per damage taken.</t>
+  </si>
+  <si>
+    <t>Gain 1 Worker recruitment per damage taken</t>
+  </si>
+  <si>
+    <t>ASSW</t>
+  </si>
+  <si>
+    <t>AASW</t>
+  </si>
+  <si>
+    <t>PPPS</t>
+  </si>
+  <si>
+    <t>PPSS</t>
+  </si>
+  <si>
+    <t>AAWW</t>
+  </si>
+  <si>
+    <t>AWWW</t>
+  </si>
+  <si>
+    <t>FPPP</t>
+  </si>
+  <si>
+    <t>SSSW</t>
+  </si>
+  <si>
+    <t>LLLMRRR</t>
+  </si>
+  <si>
+    <t>LLLRRRR</t>
+  </si>
+  <si>
+    <t>LLRRRRR</t>
+  </si>
+  <si>
+    <t>LLLLRRR</t>
+  </si>
+  <si>
+    <t>LMMMRRR</t>
+  </si>
+  <si>
+    <t>LLMMRRR</t>
+  </si>
+  <si>
+    <t>LLMRRRR</t>
+  </si>
+  <si>
+    <t>LMRRRRR</t>
+  </si>
+  <si>
+    <t>LMMRRRR</t>
+  </si>
+  <si>
+    <t>AFPP</t>
+  </si>
+  <si>
+    <t>PSSW</t>
+  </si>
+  <si>
+    <t>PWWW</t>
+  </si>
+  <si>
+    <t>FPWW</t>
+  </si>
+  <si>
+    <t>AAPS</t>
+  </si>
+  <si>
+    <t>PPSW</t>
+  </si>
+  <si>
+    <t>AAPP</t>
+  </si>
+  <si>
+    <t>AFSS</t>
+  </si>
+  <si>
+    <t>APPS</t>
+  </si>
+  <si>
+    <t>AFPW</t>
+  </si>
+  <si>
+    <t>FWWW</t>
+  </si>
+  <si>
+    <t>FPPW</t>
+  </si>
+  <si>
+    <t>APSS</t>
+  </si>
+  <si>
+    <t>APSW</t>
   </si>
 </sst>
 </file>
@@ -824,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,75 +840,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -921,26 +917,29 @@
         <v>88</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -949,126 +948,143 @@
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="C12" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C14" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>129</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1078,474 +1094,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B6252E-F41C-446B-BF8D-A5E0288C8907}">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB5132E-BDBD-4B66-8BCB-756CC0963048}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="8.7265625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="str">
-        <f>B2&amp;C2</f>
-        <v>A1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="str">
-        <f t="shared" ref="A3:A37" si="0">B3&amp;C3</f>
-        <v>B1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>A2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>B2</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>A3</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>B3</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C3</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D3</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F3</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>A4</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>B4</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C4</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D4</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F4</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>A5</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>B5</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C5</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D5</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E5</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F5</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>A6</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>B6</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>C6</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>D6</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>E6</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>F6</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB5132E-BDBD-4B66-8BCB-756CC0963048}">
-  <dimension ref="A1:D48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1555,373 +1109,355 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>107</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>108</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>109</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>108</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>110</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>111</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>107</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>109</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>112</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>109</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE23D17-6C0D-456E-99EC-518CC53A97E5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1940,15 +1476,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -1960,7 +1496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C0A2EB-FB10-4574-98A0-D1F6D1D5A86D}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1977,13 +1513,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1991,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -2002,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5">
         <v>2.5</v>
@@ -2013,7 +1549,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -2024,7 +1560,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5">
         <v>1.5</v>
@@ -2035,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5">
         <v>1.2</v>
@@ -2046,7 +1582,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -2054,10 +1590,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -2065,74 +1601,74 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>